<commit_message>
final for demo 16 probably ... ?
</commit_message>
<xml_diff>
--- a/Crawler/src/demo_16/new_data.xlsx
+++ b/Crawler/src/demo_16/new_data.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-12-18" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-12-17" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,510 +445,272 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>分散采购关于安吉高铁站游客集散中心建设运营政府采购项目的废标公告</t>
+          <t>分散采购关于安吉县2021-2023年度土地及房屋建筑物业务评估服务政府采购项目的成交结果公告</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201218/41745729-74c6-458c-afac-890abae094e0.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201217/757b8c0f-e40f-4a17-8003-95736e6bcab9.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>分散采购关于杭州东站东广场中央圆柱灯箱品牌宣传服务政府采购项目的中标(成交)结果公告</t>
+          <t>自行采购2020年西南片区农村公路提升工程（深王公路、双桥至岭西）挖方路段土、石料地质调查报告编制服务采购项目竞争性磋商</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201218/ce304cc5-b0dd-44ce-969c-1b2db3b42706.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201217/692213c9-4053-4099-b746-23bfb3c366b3.html</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>自行采购关于安吉县天子湖镇高禹村“数字高禹”建设采购项目的成交结果公告</t>
+          <t>自行采购关于安吉县智慧城市二期建设项目——安吉全域智慧旅游建设（一期）采购项目中标结果公告</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201218/cc2962ed-e206-42bb-b897-10e5d46b922f.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201217/eed0b312-740a-4c33-a083-063ad00fe62d.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>自行采购关于天荒坪镇港口村林下经济喷灌工程采购项目（第三次）的成交结果公告</t>
+          <t>自行采购关于安吉县经五路（胜利东路-芜园东路）等道路交通设施采购、安装施工工程的更正公告</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201218/f0610466-0b81-494c-95dd-e06b5faef4ac.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009003/20201217/569e1318-7784-4fd2-8392-f19a6f44079f.html</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>分散采购关于安吉智慧旅游大数据平台和网吧监测联网应急告急系统智慧平台建设政府采购项目的中标(成交)结果公告</t>
+          <t>自行采购关于安吉县经五路（胜利东路-芜园东路）等道路交通设施采购、安装施工工程的公开招标公告</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201218/e4a2fcba-27f8-40b2-bb52-9b2388c4ace5.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201217/42cffb83-9bc6-4d31-80e9-e1dd7b28f04e.html</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>自行采购关于安吉县昌硕街道穆王城社区卫生保洁服务采购项目的竞争性磋商公告</t>
+          <t>自行采购安吉中诚招标代理有限公司关于安吉县交通投资发展集团有限公司“十四五”规划编制服务采购项目的磋商公告（第二次）</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/f51bf119-6af4-4040-979e-58fb82a1b804.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201217/6fdbf2c2-c838-46a6-91b2-cf4eec51fc98.html</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>自行采购关于浙江新兴工贸有限责任公司采茶劳务采购的招标公告</t>
+          <t>自行采购关于安吉县现代农业公共服务中心装修设计施工一体化采购项目的中标结果公告</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/ba97b3c6-3b63-4bac-9fd6-fbf9619cc48f.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201217/e5910c20-ec37-4047-8f00-cdf90b8ec2dd.html</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>自行采购关于安吉信展家具有限公司雨污水管（非）开挖修复及疏通项目的竞争性磋商公告（二次采购）</t>
+          <t>自行采购关于安吉第一国际城消防设施改造工程项目的成交结果公告</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/391bb92f-386d-4f32-afe0-bcc944d17eda.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201217/a683c7c6-9c91-4c2c-a472-b2ecc86c1048.html</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>自行采购关于灵峰街道浒溪社区幸福邻里中心运营服务采购项目的竞争性磋商公告</t>
+          <t>分散采购关于安吉县2021-2023年度土地及房屋建筑物业务评估服务政府采购项目的成交结果公告</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/c1f7b14e-bf68-4e48-8b3f-5505d8018833.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201217/757b8c0f-e40f-4a17-8003-95736e6bcab9.html</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>自行采购关于安吉县递铺街道赵家上村各大小区绿化补苗种植及养护服务采购项目的竞争性磋商公告</t>
+          <t>自行采购2020年西南片区农村公路提升工程（深王公路、双桥至岭西）挖方路段土、石料地质调查报告编制服务采购项目竞争性磋商</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/7ea53ef1-5345-4f57-abff-71cfc0bcb000.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201217/692213c9-4053-4099-b746-23bfb3c366b3.html</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>自行采购关于安吉县递铺街道净土社区2021-2023年卫生保洁服务采购项目的竞争性磋商公告</t>
+          <t>自行采购关于安吉县智慧城市二期建设项目——安吉全域智慧旅游建设（一期）采购项目中标结果公告</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/1c5eea0a-07a2-4d40-b008-70e380f16fc6.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201217/eed0b312-740a-4c33-a083-063ad00fe62d.html</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>分散采购关于安吉县食品安全检验检测服务政府采购项目的竞争性磋商公告</t>
+          <t>自行采购关于安吉县经五路（胜利东路-芜园东路）等道路交通设施采购、安装施工工程的更正公告</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008001/20201218/86c1b3b2-f49b-4925-a549-7580a08186d1.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009003/20201217/569e1318-7784-4fd2-8392-f19a6f44079f.html</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>自行采购关于安吉县天荒坪镇2021年度流浪犬捕捉服务采购项目的废标公告</t>
+          <t>自行采购关于安吉县经五路（胜利东路-芜园东路）等道路交通设施采购、安装施工工程的公开招标公告</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201218/7de2e14b-dfac-4912-a7a5-70c08ef1af0b.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201217/42cffb83-9bc6-4d31-80e9-e1dd7b28f04e.html</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>集中采购安吉县公共资源交易中心关于安吉县孝源街道卫生院办公家具政府采购项目的中标(成交)结果公告</t>
+          <t>自行采购安吉中诚招标代理有限公司关于安吉县交通投资发展集团有限公司“十四五”规划编制服务采购项目的磋商公告（第二次）</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002007/003002007005/20201218/d951462b-23e2-48e3-8e74-3f127a883be1.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201217/6fdbf2c2-c838-46a6-91b2-cf4eec51fc98.html</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>集中采购安吉县公共资源交易中心关于安吉县杭垓镇人民政府消防皮卡车政府采购项目的废标公告</t>
+          <t>自行采购关于安吉县现代农业公共服务中心装修设计施工一体化采购项目的中标结果公告</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002007/003002007005/20201218/0477d84e-142b-4650-9a3c-143f410ea4af.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201217/e5910c20-ec37-4047-8f00-cdf90b8ec2dd.html</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2020-12-18</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>分散采购关于安吉高铁站游客集散中心建设运营政府采购项目的废标公告</t>
+          <t>自行采购关于安吉第一国际城消防设施改造工程项目的成交结果公告</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201218/41745729-74c6-458c-afac-890abae094e0.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>分散采购关于杭州东站东广场中央圆柱灯箱品牌宣传服务政府采购项目的中标(成交)结果公告</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201218/ce304cc5-b0dd-44ce-969c-1b2db3b42706.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>自行采购关于安吉县天子湖镇高禹村“数字高禹”建设采购项目的成交结果公告</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201218/cc2962ed-e206-42bb-b897-10e5d46b922f.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>自行采购关于天荒坪镇港口村林下经济喷灌工程采购项目（第三次）的成交结果公告</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201218/f0610466-0b81-494c-95dd-e06b5faef4ac.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>分散采购关于安吉智慧旅游大数据平台和网吧监测联网应急告急系统智慧平台建设政府采购项目的中标(成交)结果公告</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008005/20201218/e4a2fcba-27f8-40b2-bb52-9b2388c4ace5.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>自行采购关于安吉县昌硕街道穆王城社区卫生保洁服务采购项目的竞争性磋商公告</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/f51bf119-6af4-4040-979e-58fb82a1b804.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>自行采购关于浙江新兴工贸有限责任公司采茶劳务采购的招标公告</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/ba97b3c6-3b63-4bac-9fd6-fbf9619cc48f.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>自行采购关于安吉信展家具有限公司雨污水管（非）开挖修复及疏通项目的竞争性磋商公告（二次采购）</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/391bb92f-386d-4f32-afe0-bcc944d17eda.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>自行采购关于灵峰街道浒溪社区幸福邻里中心运营服务采购项目的竞争性磋商公告</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/c1f7b14e-bf68-4e48-8b3f-5505d8018833.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>自行采购关于安吉县递铺街道赵家上村各大小区绿化补苗种植及养护服务采购项目的竞争性磋商公告</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/7ea53ef1-5345-4f57-abff-71cfc0bcb000.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>自行采购关于安吉县递铺街道净土社区2021-2023年卫生保洁服务采购项目的竞争性磋商公告</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009001/20201218/1c5eea0a-07a2-4d40-b008-70e380f16fc6.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>分散采购关于安吉县食品安全检验检测服务政府采购项目的竞争性磋商公告</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002008/003002008001/20201218/86c1b3b2-f49b-4925-a549-7580a08186d1.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>自行采购关于安吉县天荒坪镇2021年度流浪犬捕捉服务采购项目的废标公告</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201218/7de2e14b-dfac-4912-a7a5-70c08ef1af0b.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>集中采购安吉县公共资源交易中心关于安吉县孝源街道卫生院办公家具政府采购项目的中标(成交)结果公告</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002007/003002007005/20201218/d951462b-23e2-48e3-8e74-3f127a883be1.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>集中采购安吉县公共资源交易中心关于安吉县杭垓镇人民政府消防皮卡车政府采购项目的废标公告</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>http://www.ajztb.com/jyxx/003002/003002007/003002007005/20201218/0477d84e-142b-4650-9a3c-143f410ea4af.html</t>
+          <t>http://www.ajztb.com/jyxx/003002/003002009/003002009005/20201217/a683c7c6-9c91-4c2c-a472-b2ecc86c1048.html</t>
         </is>
       </c>
     </row>

</xml_diff>